<commit_message>
Apport de modifications sur la feuille introduction
</commit_message>
<xml_diff>
--- a/data/Introduction.xlsx
+++ b/data/Introduction.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="48">
   <si>
     <t xml:space="preserve">Numero</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Choix</t>
   </si>
   <si>
+    <t xml:space="preserve">Style</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quel est votre rôle au sein de la collectivité ?</t>
   </si>
   <si>
@@ -44,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select</t>
   </si>
   <si>
     <t xml:space="preserve">Agent</t>
@@ -131,6 +137,9 @@
     <t xml:space="preserve">&lt; 20 000 Habitants</t>
   </si>
   <si>
+    <t xml:space="preserve">radio</t>
+  </si>
+  <si>
     <t xml:space="preserve">20 000-50 000 Habitants</t>
   </si>
   <si>
@@ -146,10 +155,16 @@
     <t xml:space="preserve">Pas obligatoire</t>
   </si>
   <si>
+    <t xml:space="preserve">checkbox</t>
+  </si>
+  <si>
     <t xml:space="preserve">Territoire littoral</t>
   </si>
   <si>
     <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucune(s)</t>
   </si>
 </sst>
 </file>
@@ -166,6 +181,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -210,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -220,13 +236,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
@@ -258,11 +267,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
@@ -279,10 +292,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -293,10 +302,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -323,6 +328,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -330,71 +441,76 @@
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="56.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="16.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="56.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="14.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -402,189 +518,209 @@
       <c r="B4" s="8"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="9"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="9" t="n">
         <v>1.1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="G5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="9" t="n">
         <v>1.1</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="9" t="n">
         <v>1.1</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="9" t="n">
         <v>1.1</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="9"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="n">
+      <c r="A10" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="G10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="n">
+      <c r="A14" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="n">
+      <c r="A15" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -597,63 +733,69 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="n">
+      <c r="A17" s="9" t="n">
         <v>1.3</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="G17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="n">
+      <c r="A18" s="9" t="n">
         <v>1.3</v>
       </c>
       <c r="B18" s="8"/>
-      <c r="C18" s="11" t="s">
-        <v>21</v>
+      <c r="C18" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="11" t="s">
-        <v>21</v>
-      </c>
       <c r="D19" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
       <c r="E20" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="6"/>
@@ -668,146 +810,162 @@
       <c r="G21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+      <c r="F22" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="G22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
       <c r="E30" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="6"/>
@@ -831,61 +989,67 @@
       <c r="G32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="3"/>
       <c r="C33" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="G33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="G34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="G35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
       <c r="E36" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="6"/>
@@ -909,91 +1073,63 @@
       <c r="G38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F39" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="G39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D40" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="6"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="D41" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="E41" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F41" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G41" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Correction pb conditions sur plusieurs questions
</commit_message>
<xml_diff>
--- a/data/Introduction.xlsx
+++ b/data/Introduction.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="49">
   <si>
     <t xml:space="preserve">Numero</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Condition</t>
   </si>
   <si>
+    <t xml:space="preserve">Parent</t>
+  </si>
+  <si>
     <t xml:space="preserve">Questions</t>
   </si>
   <si>
@@ -125,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">Une Région</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une commune, Une communauté de communes, Un syndicat mixte</t>
   </si>
   <si>
     <t xml:space="preserve">Indiquez le nombre approximatif d’habitants de votre collectivité parmi
@@ -173,7 +179,7 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -213,6 +219,11 @@
       <name val="Calibri Light"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri Light"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -264,7 +275,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -313,6 +324,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -325,14 +340,120 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -340,9 +461,10 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="56.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="16.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="14.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="56.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="14.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -352,338 +474,382 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="C4" s="8"/>
       <c r="D4" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="6"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
         <v>1.1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="n">
         <v>1.1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="6"/>
+      <c r="E7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="n">
         <v>1.1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="n">
         <v>1.1</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="n">
         <v>1.1</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9"/>
       <c r="B11" s="8"/>
-      <c r="C11" s="7"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="6"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="7" t="s">
+      <c r="C12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C13" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="D13" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C14" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="D14" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C15" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="D15" s="7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C16" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="D16" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C17" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="D17" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C18" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="D18" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
@@ -692,276 +858,300 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
-      <c r="G19" s="6"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="n">
         <v>1.3</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="6"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="n">
         <v>1.3</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="6"/>
+      <c r="E21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="n">
         <v>1.3</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="C22" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="n">
         <v>1.3</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="C23" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="6"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="6"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="C26" s="8"/>
       <c r="D26" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="6"/>
+      <c r="E26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B27" s="8"/>
-      <c r="C27" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="C27" s="8"/>
       <c r="D27" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B28" s="8"/>
-      <c r="C28" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="C28" s="8"/>
       <c r="D28" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B29" s="8"/>
-      <c r="C29" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="C29" s="8"/>
       <c r="D29" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B30" s="8"/>
-      <c r="C30" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="C30" s="8"/>
       <c r="D30" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="C31" s="8"/>
       <c r="D31" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B32" s="8"/>
-      <c r="C32" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="C32" s="8"/>
       <c r="D32" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B33" s="8"/>
-      <c r="C33" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="C33" s="8"/>
       <c r="D33" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
-      <c r="C34" s="4"/>
+      <c r="C34" s="8"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="6"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="8"/>
@@ -970,7 +1160,8 @@
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
-      <c r="G35" s="6"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="8"/>
@@ -979,73 +1170,90 @@
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
-      <c r="G36" s="6"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="7" t="s">
-        <v>35</v>
+      <c r="B37" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="7" t="n">
+        <v>2</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G37" s="6"/>
+      <c r="E37" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="7" t="s">
-        <v>35</v>
+      <c r="B38" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="7" t="n">
+        <v>2</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G38" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="7" t="s">
-        <v>35</v>
+      <c r="B39" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="7" t="n">
+        <v>2</v>
       </c>
       <c r="D39" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
-      <c r="C40" s="4"/>
+      <c r="C40" s="8"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="6"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="8"/>
@@ -1054,7 +1262,8 @@
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
-      <c r="G41" s="6"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="8"/>
@@ -1063,64 +1272,68 @@
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
-      <c r="G42" s="6"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B43" s="8"/>
-      <c r="C43" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="C43" s="8"/>
       <c r="D43" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G43" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B44" s="8"/>
-      <c r="C44" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="C44" s="8"/>
       <c r="D44" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E44" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="n">
         <v>4</v>
       </c>
       <c r="B45" s="8"/>
-      <c r="C45" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E45" s="7" t="s">
+      <c r="C45" s="8"/>
+      <c r="D45" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>